<commit_message>
work on other species
</commit_message>
<xml_diff>
--- a/tables/TableS2_species_sample_size.xlsx
+++ b/tables/TableS2_species_sample_size.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cfree/Dropbox/Chris/UCSB/projects/domoic_acid_mgmt/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC012963-2B74-834E-A16A-2D5D6C90AB5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2546AFCD-A621-E34A-ADDD-80A5FC3AB0D9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7220" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableSX_species_sample_size" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="64">
   <si>
     <t>Dungeness crab (Metacarcinus magister)</t>
   </si>
@@ -173,13 +173,52 @@
   </si>
   <si>
     <t># of samples</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Dungeness crab</t>
+  </si>
+  <si>
+    <t>California mussel</t>
+  </si>
+  <si>
+    <t>Razor clam</t>
+  </si>
+  <si>
+    <t>Rock crab</t>
+  </si>
+  <si>
+    <t>Pacific oyster</t>
+  </si>
+  <si>
+    <t>Bay mussel</t>
+  </si>
+  <si>
+    <t>Spiny lobster</t>
+  </si>
+  <si>
+    <t>Sardine/anchovy</t>
+  </si>
+  <si>
+    <t>Other crab</t>
+  </si>
+  <si>
+    <t>Other fish</t>
+  </si>
+  <si>
+    <t>Other mollusc</t>
+  </si>
+  <si>
+    <t>Other/unknown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -310,6 +349,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -667,9 +713,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1025,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,9 +1083,10 @@
     <col min="1" max="1" width="46.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -1048,8 +1096,11 @@
       <c r="C1" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1059,8 +1110,11 @@
       <c r="C2">
         <v>6237</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1070,8 +1124,11 @@
       <c r="C3">
         <v>3733</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1081,8 +1138,11 @@
       <c r="C4">
         <v>2783</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1092,8 +1152,11 @@
       <c r="C5">
         <v>1458</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1103,8 +1166,11 @@
       <c r="C6">
         <v>901</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1114,8 +1180,11 @@
       <c r="C7">
         <v>538</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1125,8 +1194,11 @@
       <c r="C8">
         <v>185</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1136,8 +1208,11 @@
       <c r="C9">
         <v>109</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1147,8 +1222,11 @@
       <c r="C10">
         <v>80</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -1158,8 +1236,11 @@
       <c r="C11">
         <v>68</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1169,8 +1250,11 @@
       <c r="C12">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -1180,8 +1264,11 @@
       <c r="C13">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1191,8 +1278,11 @@
       <c r="C14">
         <v>33</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -1202,8 +1292,11 @@
       <c r="C15">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -1213,8 +1306,11 @@
       <c r="C16">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -1224,8 +1320,11 @@
       <c r="C17">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1235,8 +1334,11 @@
       <c r="C18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1246,8 +1348,11 @@
       <c r="C19">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1257,8 +1362,11 @@
       <c r="C20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>30</v>
       </c>
@@ -1268,8 +1376,11 @@
       <c r="C21">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1279,8 +1390,11 @@
       <c r="C22">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1290,8 +1404,11 @@
       <c r="C23">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1301,8 +1418,11 @@
       <c r="C24">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1312,8 +1432,11 @@
       <c r="C25">
         <v>8</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -1323,8 +1446,11 @@
       <c r="C26">
         <v>8</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1334,8 +1460,11 @@
       <c r="C27">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1345,8 +1474,11 @@
       <c r="C28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1356,8 +1488,11 @@
       <c r="C29">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -1367,8 +1502,11 @@
       <c r="C30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -1378,8 +1516,11 @@
       <c r="C31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -1389,8 +1530,11 @@
       <c r="C32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -1400,8 +1544,11 @@
       <c r="C33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D33" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -1411,8 +1558,11 @@
       <c r="C34">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1422,8 +1572,11 @@
       <c r="C35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1433,8 +1586,11 @@
       <c r="C36">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1444,8 +1600,11 @@
       <c r="C37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1455,8 +1614,11 @@
       <c r="C38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1466,8 +1628,11 @@
       <c r="C39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -1477,8 +1642,11 @@
       <c r="C40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>46</v>
       </c>
@@ -1488,8 +1656,11 @@
       <c r="C41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1498,6 +1669,9 @@
       </c>
       <c r="C42">
         <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>